<commit_message>
Implementado hasta el % de repetibilidad
Implementado hasta el % de repetibilidad
</commit_message>
<xml_diff>
--- a/Libro1.xlsx
+++ b/Libro1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pedro\Developer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pedro\Developer\Estudio de Repitibilidad y Reproducibilidad\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -374,7 +374,7 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="A17" sqref="A17:D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -574,6 +574,7 @@
       <c r="D14">
         <v>300.60000000000002</v>
       </c>
+      <c r="G14" s="1"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">

</xml_diff>